<commit_message>
56. Highcharts column (gráfico de barras
</commit_message>
<xml_diff>
--- a/public/TimesOfCourses.xlsx
+++ b/public/TimesOfCourses.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\my-appointments\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="23580" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId5"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="73">
   <si>
     <t>Sección</t>
   </si>
@@ -224,14 +227,29 @@
   </si>
   <si>
     <t>Curso Intensivo Laravel y Android</t>
+  </si>
+  <si>
+    <t>Sección 07: Laravel: Gráficos con JS</t>
+  </si>
+  <si>
+    <t>54. Introducción a los reportes gráficos</t>
+  </si>
+  <si>
+    <t>55. Highcharts line (gráfico de líneas)</t>
+  </si>
+  <si>
+    <t>56. Highcharts column (gráfico de barras)</t>
+  </si>
+  <si>
+    <t>57. Seeder de Appointments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -290,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,27 +326,31 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ruiz Ramirez, Jose Edenilson" refreshedDate="43781.572714930553" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="53">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Edenilson Ruiz" refreshedDate="43781.909808912038" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="57">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabla1"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="SectionId" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="7"/>
     </cacheField>
     <cacheField name="SectionName" numFmtId="0">
-      <sharedItems count="12">
+      <sharedItems count="13">
         <s v="Sección 01: Introducción"/>
         <s v="Sección 02: Laravel: Configuración y Diseño Inicial"/>
         <s v="Sección 03: Laravel: Gestión de datos"/>
         <s v="Sección 04: Laravel: Roles y seguridad"/>
         <s v="Sección 05: Laravel: Horarios, citas y especialidades"/>
         <s v="Sección 06: Laravel: Estados de una cita"/>
+        <s v="Sección 07: Laravel: Gráficos con JS"/>
         <s v="Sección 4: Laravel: Roles y seguridad" u="1"/>
         <s v="Sección 2: Laravel: Configuración y Diseño Inicial" u="1"/>
         <s v="Sección 3: Laravel: Gestión de datos" u="1"/>
@@ -338,10 +360,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="ClassNumber" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="53"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="57"/>
     </cacheField>
     <cacheField name="ClassName" numFmtId="0">
-      <sharedItems count="106">
+      <sharedItems count="110">
         <s v="01. Bienvenida y recomendaciones"/>
         <s v="02. Mockups (planteamiento inicial)"/>
         <s v="03. Laravel: Configuración Inicial"/>
@@ -395,6 +417,10 @@
         <s v="51. Include según el rol de usuario"/>
         <s v="52. Detalles de citas para el rol"/>
         <s v="53. Confirmar cita"/>
+        <s v="54. Introducción a los reportes gráficos"/>
+        <s v="55. Highcharts line (gráfico de líneas)"/>
+        <s v="56. Highcharts column (gráfico de barras)"/>
+        <s v="57. Seeder de Appointments"/>
         <s v="Menú por rol" u="1"/>
         <s v="Selección múltiple en un &lt;select&gt;" u="1"/>
         <s v="Layout general para las vistas de Panel" u="1"/>
@@ -451,7 +477,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Time" numFmtId="21">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:02:00" maxDate="1899-12-30T01:05:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:00:00" maxDate="1899-12-30T01:05:00"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -463,7 +489,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="53">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="57">
   <r>
     <n v="1"/>
     <x v="0"/>
@@ -835,87 +861,116 @@
     <x v="52"/>
     <d v="1899-12-30T00:16:00"/>
   </r>
+  <r>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="54"/>
+    <x v="53"/>
+    <d v="1899-12-30T00:09:00"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="55"/>
+    <x v="54"/>
+    <d v="1899-12-30T00:26:00"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="56"/>
+    <x v="55"/>
+    <d v="1899-12-30T00:41:00"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="57"/>
+    <x v="56"/>
+    <d v="1899-12-30T00:00:00"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Sección">
-  <location ref="B4:C64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Sección">
+  <location ref="B4:C69" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="13">
+      <items count="14">
+        <item m="1" x="11"/>
+        <item m="1" x="8"/>
+        <item m="1" x="9"/>
+        <item m="1" x="7"/>
+        <item m="1" x="12"/>
         <item m="1" x="10"/>
-        <item m="1" x="7"/>
-        <item m="1" x="8"/>
-        <item m="1" x="6"/>
-        <item m="1" x="11"/>
-        <item m="1" x="9"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="106">
-        <item m="1" x="70"/>
-        <item m="1" x="97"/>
-        <item m="1" x="81"/>
-        <item m="1" x="57"/>
-        <item m="1" x="63"/>
-        <item m="1" x="92"/>
-        <item m="1" x="90"/>
-        <item m="1" x="84"/>
-        <item m="1" x="62"/>
-        <item m="1" x="88"/>
-        <item m="1" x="59"/>
-        <item m="1" x="86"/>
-        <item m="1" x="94"/>
-        <item m="1" x="65"/>
-        <item m="1" x="76"/>
-        <item m="1" x="98"/>
-        <item m="1" x="64"/>
-        <item m="1" x="71"/>
-        <item m="1" x="58"/>
-        <item m="1" x="103"/>
-        <item m="1" x="102"/>
-        <item m="1" x="91"/>
-        <item m="1" x="96"/>
-        <item m="1" x="55"/>
-        <item m="1" x="78"/>
-        <item m="1" x="77"/>
-        <item m="1" x="73"/>
-        <item m="1" x="68"/>
-        <item m="1" x="53"/>
-        <item m="1" x="104"/>
-        <item m="1" x="69"/>
-        <item m="1" x="93"/>
-        <item m="1" x="95"/>
-        <item m="1" x="82"/>
-        <item m="1" x="72"/>
-        <item m="1" x="83"/>
-        <item m="1" x="66"/>
-        <item m="1" x="100"/>
+      <items count="110">
+        <item m="1" x="74"/>
         <item m="1" x="101"/>
         <item m="1" x="85"/>
+        <item m="1" x="61"/>
+        <item m="1" x="67"/>
+        <item m="1" x="96"/>
+        <item m="1" x="94"/>
+        <item m="1" x="88"/>
+        <item m="1" x="66"/>
+        <item m="1" x="92"/>
+        <item m="1" x="63"/>
+        <item m="1" x="90"/>
+        <item m="1" x="98"/>
+        <item m="1" x="69"/>
+        <item m="1" x="80"/>
+        <item m="1" x="102"/>
+        <item m="1" x="68"/>
+        <item m="1" x="75"/>
+        <item m="1" x="62"/>
+        <item m="1" x="107"/>
+        <item m="1" x="106"/>
+        <item m="1" x="95"/>
+        <item m="1" x="100"/>
+        <item m="1" x="59"/>
+        <item m="1" x="82"/>
+        <item m="1" x="81"/>
+        <item m="1" x="77"/>
+        <item m="1" x="72"/>
+        <item m="1" x="57"/>
+        <item m="1" x="108"/>
+        <item m="1" x="73"/>
+        <item m="1" x="97"/>
+        <item m="1" x="99"/>
+        <item m="1" x="86"/>
+        <item m="1" x="76"/>
+        <item m="1" x="87"/>
+        <item m="1" x="70"/>
+        <item m="1" x="104"/>
+        <item m="1" x="105"/>
+        <item m="1" x="89"/>
+        <item m="1" x="83"/>
+        <item m="1" x="71"/>
+        <item m="1" x="91"/>
+        <item m="1" x="103"/>
+        <item m="1" x="78"/>
+        <item m="1" x="65"/>
+        <item m="1" x="58"/>
+        <item m="1" x="64"/>
+        <item m="1" x="109"/>
         <item m="1" x="79"/>
-        <item m="1" x="67"/>
-        <item m="1" x="87"/>
-        <item m="1" x="99"/>
-        <item m="1" x="74"/>
-        <item m="1" x="61"/>
-        <item m="1" x="54"/>
+        <item m="1" x="84"/>
+        <item m="1" x="93"/>
         <item m="1" x="60"/>
-        <item m="1" x="105"/>
-        <item m="1" x="75"/>
-        <item m="1" x="80"/>
-        <item m="1" x="89"/>
-        <item m="1" x="56"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -969,6 +1024,10 @@
         <item x="50"/>
         <item x="51"/>
         <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
       </items>
     </pivotField>
     <pivotField dataField="1" numFmtId="21" showAll="0"/>
@@ -977,7 +1036,7 @@
     <field x="1"/>
     <field x="3"/>
   </rowFields>
-  <rowItems count="60">
+  <rowItems count="65">
     <i>
       <x v="6"/>
     </i>
@@ -1154,6 +1213,21 @@
     </i>
     <i r="1">
       <x v="105"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="106"/>
+    </i>
+    <i r="1">
+      <x v="107"/>
+    </i>
+    <i r="1">
+      <x v="108"/>
+    </i>
+    <i r="1">
+      <x v="109"/>
     </i>
     <i t="grand">
       <x/>
@@ -1163,7 +1237,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="TiempoInvertido" fld="4" baseField="1" baseItem="0" numFmtId="165"/>
+    <dataField name="TiempoInvertido" fld="4" baseField="1" baseItem="0" numFmtId="164"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight13" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1175,7 +1249,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E54" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E58" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="SectionId"/>
     <tableColumn id="5" name="SectionName"/>
@@ -1230,7 +1304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1265,7 +1339,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1474,15 +1548,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C64"/>
+  <dimension ref="B2:C69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B59" activeCellId="5" sqref="B6:B7 B9:B18 B20:B30 B32:B34 B36:B52 B54:B63 B65:B68"/>
+      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" dimension="1" activeRow="58" activeCol="1" previousRow="58" previousCol="1" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+          <references count="1">
+            <reference field="3" count="0"/>
+          </references>
+        </pivotArea>
+      </pivotSelection>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="51" width="8.140625" customWidth="1"/>
     <col min="52" max="52" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1975,10 +2058,50 @@
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="5">
+        <v>5.2777777777777778E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="5">
+        <v>6.2499999999999995E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="5">
+        <v>1.8055555555555557E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" s="5">
+        <v>2.8472222222222222E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="5">
-        <v>0.57847222222222217</v>
+      <c r="C69" s="5">
+        <v>0.63124999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1992,9 +2115,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2923,34 +3048,78 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55">
+        <v>54</v>
+      </c>
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56">
+        <v>55</v>
+      </c>
+      <c r="D56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1.8055555555555557E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2.8472222222222222E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58">
+        <v>57</v>
+      </c>
+      <c r="D58" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizando archivo excel de tiempo invertido
</commit_message>
<xml_diff>
--- a/public/TimesOfCourses.xlsx
+++ b/public/TimesOfCourses.xlsx
@@ -17,13 +17,13 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="113">
   <si>
     <t>Sección</t>
   </si>
@@ -242,6 +242,126 @@
   </si>
   <si>
     <t>57. Seeder de Appointments</t>
+  </si>
+  <si>
+    <t>58. Formato adecuado para la respuesta JSON</t>
+  </si>
+  <si>
+    <t>59. Filtro: Actualizar según rango de fechas</t>
+  </si>
+  <si>
+    <t>Sección 08: Android: Vistas</t>
+  </si>
+  <si>
+    <t>60. Instalar Android Studio</t>
+  </si>
+  <si>
+    <t>61. Creando un proyecto nuevo</t>
+  </si>
+  <si>
+    <t>62. Estructura de carpetas</t>
+  </si>
+  <si>
+    <t>63. AVD Manager</t>
+  </si>
+  <si>
+    <t>64. Diseñando una primera vista</t>
+  </si>
+  <si>
+    <t>65. RegisterActivity y fondo gradiente</t>
+  </si>
+  <si>
+    <t>66. Diseño de MenuActivity</t>
+  </si>
+  <si>
+    <t>67. Diseño de CreateAppointment</t>
+  </si>
+  <si>
+    <t>68. Pasos en el registro de citas</t>
+  </si>
+  <si>
+    <t>69. Cómo poblar un Spinner (asignar opciones)</t>
+  </si>
+  <si>
+    <t>Sección 09: Kotlin, como alternativa a Java</t>
+  </si>
+  <si>
+    <t>70. Introducción a Kotlin</t>
+  </si>
+  <si>
+    <t>71. Primer proyecto Kotlin</t>
+  </si>
+  <si>
+    <t>72. Data Classes</t>
+  </si>
+  <si>
+    <t>73. Operators</t>
+  </si>
+  <si>
+    <t>74. Extension Functions &amp; Properties</t>
+  </si>
+  <si>
+    <t>75. Inflix functions</t>
+  </si>
+  <si>
+    <t>76. Getters &amp; Setters</t>
+  </si>
+  <si>
+    <t>77. Expression, Statement &amp; Block</t>
+  </si>
+  <si>
+    <t>78. If ( como statement y como expression)</t>
+  </si>
+  <si>
+    <t>79. When</t>
+  </si>
+  <si>
+    <t>80. Null safety</t>
+  </si>
+  <si>
+    <t>81. When - Parte 2</t>
+  </si>
+  <si>
+    <t>82. For, Ranges &amp; forEach</t>
+  </si>
+  <si>
+    <t>83. Functional Programming</t>
+  </si>
+  <si>
+    <t>Sección 10: Android: DatePicker y otros detalles</t>
+  </si>
+  <si>
+    <t>84. DatePickerDialog</t>
+  </si>
+  <si>
+    <t>85. Animate layout changes</t>
+  </si>
+  <si>
+    <t>86. Agregar RadioButtons dinámicamente</t>
+  </si>
+  <si>
+    <t>87. Múltiples RadioButtons y cómo eliminarlos</t>
+  </si>
+  <si>
+    <t>88. RadioButtons en columnas</t>
+  </si>
+  <si>
+    <t>89. Fecha: formato, valor mínimo y máximo</t>
+  </si>
+  <si>
+    <t>Sección 11: Android: RecyclerView</t>
+  </si>
+  <si>
+    <t>90. RecyclerView</t>
+  </si>
+  <si>
+    <t>91. Item View XML &amp; DataSet</t>
+  </si>
+  <si>
+    <t>92. ViewHolder (Create &amp; Bind)</t>
+  </si>
+  <si>
+    <t>93. With y otros detalles</t>
   </si>
 </sst>
 </file>
@@ -298,15 +418,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -334,16 +451,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Edenilson Ruiz" refreshedDate="43781.909808912038" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="57">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Edenilson Ruiz" refreshedDate="43786.861996180553" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="93">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabla1"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="SectionId" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="7"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="11"/>
     </cacheField>
     <cacheField name="SectionName" numFmtId="0">
-      <sharedItems count="13">
+      <sharedItems count="17">
         <s v="Sección 01: Introducción"/>
         <s v="Sección 02: Laravel: Configuración y Diseño Inicial"/>
         <s v="Sección 03: Laravel: Gestión de datos"/>
@@ -351,6 +468,10 @@
         <s v="Sección 05: Laravel: Horarios, citas y especialidades"/>
         <s v="Sección 06: Laravel: Estados de una cita"/>
         <s v="Sección 07: Laravel: Gráficos con JS"/>
+        <s v="Sección 08: Android: Vistas"/>
+        <s v="Sección 09: Kotlin, como alternativa a Java"/>
+        <s v="Sección 10: Android: DatePicker y otros detalles"/>
+        <s v="Sección 11: Android: RecyclerView"/>
         <s v="Sección 4: Laravel: Roles y seguridad" u="1"/>
         <s v="Sección 2: Laravel: Configuración y Diseño Inicial" u="1"/>
         <s v="Sección 3: Laravel: Gestión de datos" u="1"/>
@@ -360,10 +481,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="ClassNumber" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="57"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="93"/>
     </cacheField>
     <cacheField name="ClassName" numFmtId="0">
-      <sharedItems count="110">
+      <sharedItems count="146">
         <s v="01. Bienvenida y recomendaciones"/>
         <s v="02. Mockups (planteamiento inicial)"/>
         <s v="03. Laravel: Configuración Inicial"/>
@@ -421,63 +542,99 @@
         <s v="55. Highcharts line (gráfico de líneas)"/>
         <s v="56. Highcharts column (gráfico de barras)"/>
         <s v="57. Seeder de Appointments"/>
+        <s v="58. Formato adecuado para la respuesta JSON"/>
+        <s v="59. Filtro: Actualizar según rango de fechas"/>
+        <s v="60. Instalar Android Studio"/>
+        <s v="61. Creando un proyecto nuevo"/>
+        <s v="62. Estructura de carpetas"/>
+        <s v="63. AVD Manager"/>
+        <s v="64. Diseñando una primera vista"/>
+        <s v="65. RegisterActivity y fondo gradiente"/>
+        <s v="66. Diseño de MenuActivity"/>
+        <s v="67. Diseño de CreateAppointment"/>
+        <s v="68. Pasos en el registro de citas"/>
+        <s v="69. Cómo poblar un Spinner (asignar opciones)"/>
+        <s v="70. Introducción a Kotlin"/>
+        <s v="71. Primer proyecto Kotlin"/>
+        <s v="72. Data Classes"/>
+        <s v="73. Operators"/>
+        <s v="74. Extension Functions &amp; Properties"/>
+        <s v="75. Inflix functions"/>
+        <s v="76. Getters &amp; Setters"/>
+        <s v="77. Expression, Statement &amp; Block"/>
+        <s v="78. If ( como statement y como expression)"/>
+        <s v="79. When"/>
+        <s v="80. Null safety"/>
+        <s v="81. When - Parte 2"/>
+        <s v="82. For, Ranges &amp; forEach"/>
+        <s v="83. Functional Programming"/>
+        <s v="84. DatePickerDialog"/>
+        <s v="85. Animate layout changes"/>
+        <s v="86. Agregar RadioButtons dinámicamente"/>
+        <s v="87. Múltiples RadioButtons y cómo eliminarlos"/>
+        <s v="88. RadioButtons en columnas"/>
+        <s v="89. Fecha: formato, valor mínimo y máximo"/>
+        <s v="90. RecyclerView"/>
+        <s v="91. Item View XML &amp; DataSet"/>
+        <s v="92. ViewHolder (Create &amp; Bind)"/>
+        <s v="93. With y otros detalles"/>
+        <s v="Cancelación de citas médicas" u="1"/>
+        <s v="Métodos update y destroy" u="1"/>
+        <s v="Directiva include y menú lateral" u="1"/>
+        <s v="Consultas según el rol de usuario" u="1"/>
+        <s v="Relación muchos a muchos" u="1"/>
+        <s v="Verbo PUT (editar especialidades)" u="1"/>
+        <s v="Seeders, Model factories y Faker" u="1"/>
+        <s v="Gestionando relaciones Many to Many" u="1"/>
+        <s v="Modelado y lógica para guardar" u="1"/>
+        <s v="Médicos según especialidad" u="1"/>
+        <s v="Selección múltiple en un &lt;select&gt;" u="1"/>
+        <s v="Select dinámico y límites al DatePicker" u="1"/>
+        <s v="Formulario: Registrar cita médica" u="1"/>
+        <s v="Detalles de cancelación" u="1"/>
+        <s v="Confirmar cita" u="1"/>
+        <s v="Verbo DELETE (eliminar especialidades)" u="1"/>
+        <s v="Radio Buttons y Alert dinámicamente" u="1"/>
+        <s v="Repositorio en Github (Proyecto Laravel)" u="1"/>
+        <s v="Organizando controladores en carpetas" u="1"/>
+        <s v="Proteger rutas usando Middlewares" u="1"/>
+        <s v="Campo status y relaciones entre modelos" u="1"/>
+        <s v="Horas de atención por intervalos" u="1"/>
+        <s v="Mass assigment y edit" u="1"/>
+        <s v="Repaso y Services Providers" u="1"/>
+        <s v="Vistas, rutas y controladores" u="1"/>
+        <s v="Diseño base para nuestra app web" u="1"/>
+        <s v="Doctor Resource" u="1"/>
         <s v="Menú por rol" u="1"/>
-        <s v="Selección múltiple en un &lt;select&gt;" u="1"/>
-        <s v="Layout general para las vistas de Panel" u="1"/>
-        <s v="Vistas, rutas y controladores" u="1"/>
-        <s v="Cancelación de citas médicas" u="1"/>
-        <s v="Gestionando relaciones Many to Many" u="1"/>
-        <s v="Directiva include y menú lateral" u="1"/>
-        <s v="Select dinámico y límites al DatePicker" u="1"/>
-        <s v="Seeders, Model factories y Faker" u="1"/>
-        <s v="Detalles de cancelación" u="1"/>
-        <s v="Citas organizadas en tabs" u="1"/>
-        <s v="Formulario de registro y menú" u="1"/>
-        <s v="Dropdown menu" u="1"/>
-        <s v="Patient Resource" u="1"/>
-        <s v="Relación muchos a muchos" u="1"/>
-        <s v="Médicos según especialidad" u="1"/>
-        <s v="Migraciones y Autenticación" u="1"/>
-        <s v="Bienvenida y recomendaciones" u="1"/>
-        <s v="Formulario: Registrar cita médica" u="1"/>
-        <s v="Múltiples directivas yield y menú" u="1"/>
-        <s v="Mass assigment y edit" u="1"/>
-        <s v="Rutas y vista (diseño inicial)" u="1"/>
-        <s v="Validaciones de lado del clientey servidor" u="1"/>
+        <s v="Include según el rol de usuario" u="1"/>
+        <s v="Validación de horas (evitar colisión)" u="1"/>
         <s v="Especialidades" u="1"/>
         <s v="Login como página de inicio" u="1"/>
+        <s v="Mostrar horario (Carbon y método map)" u="1"/>
+        <s v="Layout general para las vistas de Panel" u="1"/>
         <s v="Lógica para los estados y siguientes pasos" u="1"/>
+        <s v="Integrar plantilla Argon (Login)" u="1"/>
         <s v="Registro de cita médica (Web)" u="1"/>
-        <s v="Verbo DELETE (eliminar especialidades)" u="1"/>
-        <s v="Campo status y relaciones entre modelos" u="1"/>
-        <s v="Mostrar horario (Carbon y método map)" u="1"/>
-        <s v="Organizando controladores en carpetas" u="1"/>
-        <s v="Consultas según el rol de usuario" u="1"/>
-        <s v="Radio Buttons y Alert dinámicamente" u="1"/>
-        <s v="Diseño base para nuestra app web" u="1"/>
-        <s v="Repaso y Services Providers" u="1"/>
+        <s v="Flashed Session Data" u="1"/>
+        <s v="Migraciones y Autenticación" u="1"/>
+        <s v="Validaciones de lado del clientey servidor" u="1"/>
+        <s v="Patient Resource" u="1"/>
+        <s v="Citas organizadas en tabs" u="1"/>
+        <s v="Múltiples directivas yield y menú" u="1"/>
+        <s v="Formulario de registro y menú" u="1"/>
+        <s v="Laravel: Configuración Inicial" u="1"/>
+        <s v="Mockups (planteamiento inicial)" u="1"/>
+        <s v="Rutas y vista (diseño inicial)" u="1"/>
+        <s v="Dropdown menu" u="1"/>
+        <s v="Bienvenida y recomendaciones" u="1"/>
+        <s v="Consistencia en las horas" u="1"/>
+        <s v="Bloquear horas según reserva de citas" u="1"/>
         <s v="Detalles de citas para el rol" u="1"/>
-        <s v="Verbo PUT (editar especialidades)" u="1"/>
-        <s v="Consistencia en las horas" u="1"/>
-        <s v="Integrar plantilla Argon (Login)" u="1"/>
-        <s v="Confirmar cita" u="1"/>
-        <s v="Mockups (planteamiento inicial)" u="1"/>
-        <s v="Doctor Resource" u="1"/>
-        <s v="Modelado y lógica para guardar" u="1"/>
-        <s v="Laravel: Configuración Inicial" u="1"/>
-        <s v="Bloquear horas según reserva de citas" u="1"/>
-        <s v="Flashed Session Data" u="1"/>
-        <s v="Repositorio en Github (Proyecto Laravel)" u="1"/>
-        <s v="Proteger rutas usando Middlewares" u="1"/>
         <s v="Query Scopes" u="1"/>
-        <s v="Include según el rol de usuario" u="1"/>
-        <s v="Horas de atención por intervalos" u="1"/>
-        <s v="Métodos update y destroy" u="1"/>
-        <s v="Validación de horas (evitar colisión)" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Time" numFmtId="21">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:00:00" maxDate="1899-12-30T01:05:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:02:00" maxDate="1899-12-30T01:05:00"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -489,7 +646,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="57">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="93">
   <r>
     <n v="1"/>
     <x v="0"/>
@@ -887,90 +1044,346 @@
     <x v="6"/>
     <n v="57"/>
     <x v="56"/>
-    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T00:19:00"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="58"/>
+    <x v="57"/>
+    <d v="1899-12-30T00:12:00"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="59"/>
+    <x v="58"/>
+    <d v="1899-12-30T00:28:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="60"/>
+    <x v="59"/>
+    <d v="1899-12-30T00:03:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="61"/>
+    <x v="60"/>
+    <d v="1899-12-30T00:10:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="62"/>
+    <x v="61"/>
+    <d v="1899-12-30T00:05:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="63"/>
+    <x v="62"/>
+    <d v="1899-12-30T00:06:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="64"/>
+    <x v="63"/>
+    <d v="1899-12-30T00:32:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="65"/>
+    <x v="64"/>
+    <d v="1899-12-30T00:21:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="66"/>
+    <x v="65"/>
+    <d v="1899-12-30T00:19:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="67"/>
+    <x v="66"/>
+    <d v="1899-12-30T00:16:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="68"/>
+    <x v="67"/>
+    <d v="1899-12-30T00:14:00"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="69"/>
+    <x v="68"/>
+    <d v="1899-12-30T00:08:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="70"/>
+    <x v="69"/>
+    <d v="1899-12-30T00:10:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="71"/>
+    <x v="70"/>
+    <d v="1899-12-30T00:15:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="72"/>
+    <x v="71"/>
+    <d v="1899-12-30T00:27:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="73"/>
+    <x v="72"/>
+    <d v="1899-12-30T00:18:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="74"/>
+    <x v="73"/>
+    <d v="1899-12-30T00:12:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="75"/>
+    <x v="74"/>
+    <d v="1899-12-30T00:03:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="76"/>
+    <x v="75"/>
+    <d v="1899-12-30T00:12:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="77"/>
+    <x v="76"/>
+    <d v="1899-12-30T00:05:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="78"/>
+    <x v="77"/>
+    <d v="1899-12-30T00:11:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="79"/>
+    <x v="78"/>
+    <d v="1899-12-30T00:10:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="80"/>
+    <x v="79"/>
+    <d v="1899-12-30T00:15:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="81"/>
+    <x v="80"/>
+    <d v="1899-12-30T00:08:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="82"/>
+    <x v="81"/>
+    <d v="1899-12-30T00:13:00"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="83"/>
+    <x v="82"/>
+    <d v="1899-12-30T00:25:00"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="9"/>
+    <n v="84"/>
+    <x v="83"/>
+    <d v="1899-12-30T00:15:00"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="9"/>
+    <n v="85"/>
+    <x v="84"/>
+    <d v="1899-12-30T00:02:00"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="9"/>
+    <n v="86"/>
+    <x v="85"/>
+    <d v="1899-12-30T00:05:00"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="9"/>
+    <n v="87"/>
+    <x v="86"/>
+    <d v="1899-12-30T00:03:00"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="9"/>
+    <n v="88"/>
+    <x v="87"/>
+    <d v="1899-12-30T00:18:00"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="9"/>
+    <n v="89"/>
+    <x v="88"/>
+    <d v="1899-12-30T00:14:00"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="10"/>
+    <n v="90"/>
+    <x v="89"/>
+    <d v="1899-12-30T00:14:00"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="10"/>
+    <n v="91"/>
+    <x v="90"/>
+    <d v="1899-12-30T00:22:00"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="10"/>
+    <n v="92"/>
+    <x v="91"/>
+    <d v="1899-12-30T00:10:00"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="10"/>
+    <n v="93"/>
+    <x v="92"/>
+    <d v="1899-12-30T00:12:00"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Sección">
-  <location ref="B4:C69" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Sección">
+  <location ref="B4:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="14">
-        <item m="1" x="11"/>
-        <item m="1" x="8"/>
-        <item m="1" x="9"/>
-        <item m="1" x="7"/>
-        <item m="1" x="12"/>
-        <item m="1" x="10"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item t="default"/>
+      <items count="18">
+        <item sd="0" m="1" x="15"/>
+        <item sd="0" m="1" x="12"/>
+        <item sd="0" m="1" x="13"/>
+        <item sd="0" m="1" x="11"/>
+        <item sd="0" m="1" x="16"/>
+        <item sd="0" m="1" x="14"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item t="default" sd="0"/>
       </items>
     </pivotField>
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="110">
-        <item m="1" x="74"/>
+      <items count="146">
+        <item m="1" x="141"/>
+        <item m="1" x="143"/>
+        <item m="1" x="113"/>
+        <item m="1" x="93"/>
+        <item m="1" x="134"/>
+        <item m="1" x="107"/>
+        <item m="1" x="142"/>
+        <item m="1" x="96"/>
+        <item m="1" x="106"/>
+        <item m="1" x="144"/>
+        <item m="1" x="95"/>
+        <item m="1" x="118"/>
+        <item m="1" x="119"/>
+        <item m="1" x="140"/>
+        <item m="1" x="123"/>
+        <item m="1" x="130"/>
+        <item m="1" x="136"/>
+        <item m="1" x="105"/>
+        <item m="1" x="100"/>
+        <item m="1" x="114"/>
+        <item m="1" x="121"/>
+        <item m="1" x="128"/>
+        <item m="1" x="137"/>
+        <item m="1" x="126"/>
+        <item m="1" x="127"/>
+        <item m="1" x="124"/>
+        <item m="1" x="115"/>
+        <item m="1" x="102"/>
+        <item m="1" x="120"/>
+        <item m="1" x="94"/>
+        <item m="1" x="131"/>
+        <item m="1" x="138"/>
         <item m="1" x="101"/>
-        <item m="1" x="85"/>
-        <item m="1" x="61"/>
-        <item m="1" x="67"/>
-        <item m="1" x="96"/>
-        <item m="1" x="94"/>
-        <item m="1" x="88"/>
-        <item m="1" x="66"/>
-        <item m="1" x="92"/>
-        <item m="1" x="63"/>
-        <item m="1" x="90"/>
+        <item m="1" x="125"/>
+        <item m="1" x="135"/>
+        <item m="1" x="111"/>
+        <item m="1" x="133"/>
+        <item m="1" x="112"/>
+        <item m="1" x="145"/>
+        <item m="1" x="109"/>
+        <item m="1" x="129"/>
+        <item m="1" x="97"/>
+        <item m="1" x="116"/>
+        <item m="1" x="110"/>
+        <item m="1" x="139"/>
+        <item m="1" x="99"/>
+        <item m="1" x="103"/>
+        <item m="1" x="104"/>
+        <item m="1" x="122"/>
+        <item m="1" x="132"/>
+        <item m="1" x="108"/>
         <item m="1" x="98"/>
-        <item m="1" x="69"/>
-        <item m="1" x="80"/>
-        <item m="1" x="102"/>
-        <item m="1" x="68"/>
-        <item m="1" x="75"/>
-        <item m="1" x="62"/>
-        <item m="1" x="107"/>
-        <item m="1" x="106"/>
-        <item m="1" x="95"/>
-        <item m="1" x="100"/>
-        <item m="1" x="59"/>
-        <item m="1" x="82"/>
-        <item m="1" x="81"/>
-        <item m="1" x="77"/>
-        <item m="1" x="72"/>
-        <item m="1" x="57"/>
-        <item m="1" x="108"/>
-        <item m="1" x="73"/>
-        <item m="1" x="97"/>
-        <item m="1" x="99"/>
-        <item m="1" x="86"/>
-        <item m="1" x="76"/>
-        <item m="1" x="87"/>
-        <item m="1" x="70"/>
-        <item m="1" x="104"/>
-        <item m="1" x="105"/>
-        <item m="1" x="89"/>
-        <item m="1" x="83"/>
-        <item m="1" x="71"/>
-        <item m="1" x="91"/>
-        <item m="1" x="103"/>
-        <item m="1" x="78"/>
-        <item m="1" x="65"/>
-        <item m="1" x="58"/>
-        <item m="1" x="64"/>
-        <item m="1" x="109"/>
-        <item m="1" x="79"/>
-        <item m="1" x="84"/>
-        <item m="1" x="93"/>
-        <item m="1" x="60"/>
+        <item m="1" x="117"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1028,6 +1441,42 @@
         <item x="54"/>
         <item x="55"/>
         <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
       </items>
     </pivotField>
     <pivotField dataField="1" numFmtId="21" showAll="0"/>
@@ -1036,198 +1485,39 @@
     <field x="1"/>
     <field x="3"/>
   </rowFields>
-  <rowItems count="65">
+  <rowItems count="12">
     <i>
       <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="53"/>
-    </i>
-    <i r="1">
-      <x v="54"/>
     </i>
     <i>
       <x v="7"/>
     </i>
-    <i r="1">
-      <x v="55"/>
-    </i>
-    <i r="1">
-      <x v="56"/>
-    </i>
-    <i r="1">
-      <x v="57"/>
-    </i>
-    <i r="1">
-      <x v="58"/>
-    </i>
-    <i r="1">
-      <x v="59"/>
-    </i>
-    <i r="1">
-      <x v="60"/>
-    </i>
-    <i r="1">
-      <x v="61"/>
-    </i>
-    <i r="1">
-      <x v="62"/>
-    </i>
-    <i r="1">
-      <x v="63"/>
-    </i>
-    <i r="1">
-      <x v="64"/>
-    </i>
     <i>
       <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="65"/>
-    </i>
-    <i r="1">
-      <x v="66"/>
-    </i>
-    <i r="1">
-      <x v="67"/>
-    </i>
-    <i r="1">
-      <x v="68"/>
-    </i>
-    <i r="1">
-      <x v="69"/>
-    </i>
-    <i r="1">
-      <x v="70"/>
-    </i>
-    <i r="1">
-      <x v="71"/>
-    </i>
-    <i r="1">
-      <x v="72"/>
-    </i>
-    <i r="1">
-      <x v="73"/>
-    </i>
-    <i r="1">
-      <x v="74"/>
-    </i>
-    <i r="1">
-      <x v="75"/>
     </i>
     <i>
       <x v="9"/>
     </i>
-    <i r="1">
-      <x v="76"/>
-    </i>
-    <i r="1">
-      <x v="77"/>
-    </i>
-    <i r="1">
-      <x v="78"/>
-    </i>
     <i>
       <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="79"/>
-    </i>
-    <i r="1">
-      <x v="80"/>
-    </i>
-    <i r="1">
-      <x v="81"/>
-    </i>
-    <i r="1">
-      <x v="82"/>
-    </i>
-    <i r="1">
-      <x v="83"/>
-    </i>
-    <i r="1">
-      <x v="84"/>
-    </i>
-    <i r="1">
-      <x v="85"/>
-    </i>
-    <i r="1">
-      <x v="86"/>
-    </i>
-    <i r="1">
-      <x v="87"/>
-    </i>
-    <i r="1">
-      <x v="88"/>
-    </i>
-    <i r="1">
-      <x v="89"/>
-    </i>
-    <i r="1">
-      <x v="90"/>
-    </i>
-    <i r="1">
-      <x v="91"/>
-    </i>
-    <i r="1">
-      <x v="92"/>
-    </i>
-    <i r="1">
-      <x v="93"/>
-    </i>
-    <i r="1">
-      <x v="94"/>
-    </i>
-    <i r="1">
-      <x v="95"/>
     </i>
     <i>
       <x v="11"/>
     </i>
-    <i r="1">
-      <x v="96"/>
-    </i>
-    <i r="1">
-      <x v="97"/>
-    </i>
-    <i r="1">
-      <x v="98"/>
-    </i>
-    <i r="1">
-      <x v="99"/>
-    </i>
-    <i r="1">
-      <x v="100"/>
-    </i>
-    <i r="1">
-      <x v="101"/>
-    </i>
-    <i r="1">
-      <x v="102"/>
-    </i>
-    <i r="1">
-      <x v="103"/>
-    </i>
-    <i r="1">
-      <x v="104"/>
-    </i>
-    <i r="1">
-      <x v="105"/>
-    </i>
     <i>
       <x v="12"/>
     </i>
-    <i r="1">
-      <x v="106"/>
+    <i>
+      <x v="13"/>
     </i>
-    <i r="1">
-      <x v="107"/>
+    <i>
+      <x v="14"/>
     </i>
-    <i r="1">
-      <x v="108"/>
+    <i>
+      <x v="15"/>
     </i>
-    <i r="1">
-      <x v="109"/>
+    <i>
+      <x v="16"/>
     </i>
     <i t="grand">
       <x/>
@@ -1249,7 +1539,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E58" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E94" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="SectionId"/>
     <tableColumn id="5" name="SectionName"/>
@@ -1548,17 +1838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C69"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B59" activeCellId="5" sqref="B6:B7 B9:B18 B20:B30 B32:B34 B36:B52 B54:B63 B65:B68"/>
-      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" dimension="1" activeRow="58" activeCol="1" previousRow="58" previousCol="1" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-          <references count="1">
-            <reference field="3" count="0"/>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,10 +1854,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1588,520 +1871,96 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2.0833333333333333E-3</v>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8.819444444444445E-2</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5">
-        <v>7.6388888888888886E-3</v>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.10694444444444445</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5">
-        <v>8.819444444444445E-2</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.5972222222222221E-2</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5">
-        <v>7.6388888888888886E-3</v>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.23958333333333334</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5">
-        <v>4.1666666666666666E-3</v>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.11805555555555555</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1.3888888888888889E-3</v>
+      <c r="B11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="4">
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5">
-        <v>4.8611111111111112E-3</v>
+      <c r="B12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9.3055555555555544E-2</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5">
-        <v>2.1527777777777781E-2</v>
+      <c r="B13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.12777777777777777</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5">
-        <v>6.2499999999999995E-3</v>
+      <c r="B14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3.9583333333333331E-2</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="5">
-        <v>7.6388888888888886E-3</v>
+      <c r="B15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4.0277777777777773E-2</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="5">
-        <v>9.7222222222222224E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1.0416666666666666E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1.4583333333333332E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0.10694444444444445</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="5">
-        <v>2.013888888888889E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="5">
-        <v>6.2499999999999995E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="5">
-        <v>9.7222222222222224E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="5">
-        <v>4.8611111111111112E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="5">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="5">
-        <v>9.7222222222222224E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="5">
-        <v>7.6388888888888886E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="5">
-        <v>1.5972222222222224E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="5">
-        <v>6.2499999999999995E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="5">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="5">
-        <v>1.5972222222222221E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="5">
-        <v>7.6388888888888886E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="5">
-        <v>5.5555555555555558E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="5">
-        <v>2.7777777777777779E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="5">
-        <v>0.23958333333333334</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="5">
-        <v>1.1111111111111112E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="5">
-        <v>1.7361111111111112E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="5">
-        <v>4.1666666666666666E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="5">
-        <v>1.1111111111111112E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="5">
-        <v>1.0416666666666666E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="5">
-        <v>8.3333333333333332E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="5">
-        <v>9.7222222222222224E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="5">
-        <v>8.3333333333333332E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="5">
-        <v>1.1111111111111112E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="5">
-        <v>1.0416666666666666E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="5">
-        <v>9.7222222222222224E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="5">
-        <v>2.1527777777777781E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="5">
-        <v>1.5972222222222224E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="5">
-        <v>4.5138888888888888E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="5">
-        <v>2.8472222222222222E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="5">
-        <v>5.5555555555555558E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="5">
-        <v>1.1111111111111112E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" s="5">
-        <v>0.11805555555555555</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="5">
-        <v>1.7361111111111112E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C55" s="5">
-        <v>1.1805555555555555E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" s="5">
-        <v>1.3888888888888888E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="5">
-        <v>2.361111111111111E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="5">
-        <v>1.3888888888888888E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C59" s="5">
-        <v>2.7777777777777779E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C60" s="5">
-        <v>1.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="5">
-        <v>4.1666666666666666E-3</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="5">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C63" s="5">
-        <v>1.1111111111111112E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C64" s="5">
-        <v>5.2777777777777778E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" s="5">
-        <v>6.2499999999999995E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="5">
-        <v>1.8055555555555557E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C67" s="5">
-        <v>2.8472222222222222E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C68" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C69" s="5">
-        <v>0.63124999999999998</v>
+      <c r="C16" s="4">
+        <v>0.97291666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -2115,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView showGridLines="0" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,7 +1985,7 @@
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3113,7 +2972,619 @@
         <v>72</v>
       </c>
       <c r="E58" s="1">
-        <v>0</v>
+        <v>1.3194444444444444E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59">
+        <v>58</v>
+      </c>
+      <c r="D59" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1.9444444444444445E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61">
+        <v>60</v>
+      </c>
+      <c r="D61" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>8</v>
+      </c>
+      <c r="B62" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62">
+        <v>61</v>
+      </c>
+      <c r="D62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63">
+        <v>62</v>
+      </c>
+      <c r="D63" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>8</v>
+      </c>
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64">
+        <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>79</v>
+      </c>
+      <c r="E64" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2.2222222222222223E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>8</v>
+      </c>
+      <c r="B66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66">
+        <v>65</v>
+      </c>
+      <c r="D66" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1.4583333333333332E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67">
+        <v>66</v>
+      </c>
+      <c r="D67" t="s">
+        <v>82</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1.3194444444444444E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>8</v>
+      </c>
+      <c r="B68" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68">
+        <v>67</v>
+      </c>
+      <c r="D68" t="s">
+        <v>83</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1.1111111111111112E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69">
+        <v>68</v>
+      </c>
+      <c r="D69" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="1">
+        <v>9.7222222222222224E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70">
+        <v>69</v>
+      </c>
+      <c r="D70" t="s">
+        <v>85</v>
+      </c>
+      <c r="E70" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71">
+        <v>70</v>
+      </c>
+      <c r="D71" t="s">
+        <v>87</v>
+      </c>
+      <c r="E71" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>9</v>
+      </c>
+      <c r="B72" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72">
+        <v>71</v>
+      </c>
+      <c r="D72" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>9</v>
+      </c>
+      <c r="B73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73">
+        <v>72</v>
+      </c>
+      <c r="D73" t="s">
+        <v>89</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1.8749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>9</v>
+      </c>
+      <c r="B74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74">
+        <v>73</v>
+      </c>
+      <c r="D74" t="s">
+        <v>90</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>9</v>
+      </c>
+      <c r="B75" t="s">
+        <v>86</v>
+      </c>
+      <c r="C75">
+        <v>74</v>
+      </c>
+      <c r="D75" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>9</v>
+      </c>
+      <c r="B76" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76">
+        <v>75</v>
+      </c>
+      <c r="D76" t="s">
+        <v>92</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>9</v>
+      </c>
+      <c r="B77" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77">
+        <v>76</v>
+      </c>
+      <c r="D77" t="s">
+        <v>93</v>
+      </c>
+      <c r="E77" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>9</v>
+      </c>
+      <c r="B78" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78">
+        <v>77</v>
+      </c>
+      <c r="D78" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>9</v>
+      </c>
+      <c r="B79" t="s">
+        <v>86</v>
+      </c>
+      <c r="C79">
+        <v>78</v>
+      </c>
+      <c r="D79" t="s">
+        <v>95</v>
+      </c>
+      <c r="E79" s="1">
+        <v>7.6388888888888886E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>9</v>
+      </c>
+      <c r="B80" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80">
+        <v>79</v>
+      </c>
+      <c r="D80" t="s">
+        <v>96</v>
+      </c>
+      <c r="E80" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>9</v>
+      </c>
+      <c r="B81" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81">
+        <v>80</v>
+      </c>
+      <c r="D81" t="s">
+        <v>97</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>9</v>
+      </c>
+      <c r="B82" t="s">
+        <v>86</v>
+      </c>
+      <c r="C82">
+        <v>81</v>
+      </c>
+      <c r="D82" t="s">
+        <v>98</v>
+      </c>
+      <c r="E82" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>9</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83">
+        <v>82</v>
+      </c>
+      <c r="D83" t="s">
+        <v>99</v>
+      </c>
+      <c r="E83" s="1">
+        <v>9.0277777777777787E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84">
+        <v>83</v>
+      </c>
+      <c r="D84" t="s">
+        <v>100</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1.7361111111111112E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85">
+        <v>84</v>
+      </c>
+      <c r="D85" t="s">
+        <v>102</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>10</v>
+      </c>
+      <c r="B86" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86">
+        <v>85</v>
+      </c>
+      <c r="D86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>10</v>
+      </c>
+      <c r="B87" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87">
+        <v>86</v>
+      </c>
+      <c r="D87" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>10</v>
+      </c>
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88">
+        <v>87</v>
+      </c>
+      <c r="D88" t="s">
+        <v>105</v>
+      </c>
+      <c r="E88" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>10</v>
+      </c>
+      <c r="B89" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89">
+        <v>88</v>
+      </c>
+      <c r="D89" t="s">
+        <v>106</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>10</v>
+      </c>
+      <c r="B90" t="s">
+        <v>101</v>
+      </c>
+      <c r="C90">
+        <v>89</v>
+      </c>
+      <c r="D90" t="s">
+        <v>107</v>
+      </c>
+      <c r="E90" s="1">
+        <v>9.7222222222222224E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>11</v>
+      </c>
+      <c r="B91" t="s">
+        <v>108</v>
+      </c>
+      <c r="C91">
+        <v>90</v>
+      </c>
+      <c r="D91" t="s">
+        <v>109</v>
+      </c>
+      <c r="E91" s="1">
+        <v>9.7222222222222224E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>11</v>
+      </c>
+      <c r="B92" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92">
+        <v>91</v>
+      </c>
+      <c r="D92" t="s">
+        <v>110</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1.5277777777777777E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>11</v>
+      </c>
+      <c r="B93" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93">
+        <v>92</v>
+      </c>
+      <c r="D93" t="s">
+        <v>111</v>
+      </c>
+      <c r="E93" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>11</v>
+      </c>
+      <c r="B94" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94">
+        <v>93</v>
+      </c>
+      <c r="D94" t="s">
+        <v>112</v>
+      </c>
+      <c r="E94" s="1">
+        <v>8.3333333333333332E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de horas invertidas
</commit_message>
<xml_diff>
--- a/public/TimesOfCourses.xlsx
+++ b/public/TimesOfCourses.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="167">
   <si>
     <t>Sección</t>
   </si>
@@ -362,16 +362,180 @@
   </si>
   <si>
     <t>93. With y otros detalles</t>
+  </si>
+  <si>
+    <t>Sección 12: Android: Navegación entre pantallas</t>
+  </si>
+  <si>
+    <t>94. Back button</t>
+  </si>
+  <si>
+    <t>95. Finalizar un Activity tras iniciar otro</t>
+  </si>
+  <si>
+    <t>96 Cómo tener una única instancia (Activity)</t>
+  </si>
+  <si>
+    <t>97. Persistencia de datos para el Login</t>
+  </si>
+  <si>
+    <t>99. Shared Preferences, usando Kotlin</t>
+  </si>
+  <si>
+    <t>98. Shared Preferences, tal como son</t>
+  </si>
+  <si>
+    <t>100. Repositorio en Github (Proyecto Android)</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://github.com/JCarlosR/MyAppointments</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/JCarlosR/7f457aeebd9c3670933221e97116c4c6</t>
+  </si>
+  <si>
+    <t>101. Snackbar by lazy</t>
+  </si>
+  <si>
+    <t>102. Alert Dialog</t>
+  </si>
+  <si>
+    <t>103. Paso previo, mensaje de error y checked</t>
+  </si>
+  <si>
+    <t>104. Mostrar datos, para Confirmar cita</t>
+  </si>
+  <si>
+    <t>105. Validar selección de fecha y hora</t>
+  </si>
+  <si>
+    <t>106. Off-topic: Cómo crear y compartir un Gif</t>
+  </si>
+  <si>
+    <t>Gifcam.zip</t>
+  </si>
+  <si>
+    <t>Sección 13: Despliegue a producción</t>
+  </si>
+  <si>
+    <t>107. Registro en Digital Ocean</t>
+  </si>
+  <si>
+    <t>https://programacionymas.com/blog/hacer-deploy-app-laravel-digital-ocean</t>
+  </si>
+  <si>
+    <t>108. Conexión vía SSH</t>
+  </si>
+  <si>
+    <t>109. Instalación de paquetes y dependencias</t>
+  </si>
+  <si>
+    <t>110. Corregir conexión MySQL</t>
+  </si>
+  <si>
+    <t>111. Comandos Git: log, status, push, pull</t>
+  </si>
+  <si>
+    <t>112. Laravel log</t>
+  </si>
+  <si>
+    <t>Sección 14: Android y Laravel: Autenticación vía JWT</t>
+  </si>
+  <si>
+    <t>113. Encoding, Encryption &amp; Hashing</t>
+  </si>
+  <si>
+    <t>114. JWT: Flujo de autenticación</t>
+  </si>
+  <si>
+    <t>115. Cómo se genera y valida un JWT (5 pasos)</t>
+  </si>
+  <si>
+    <t>116. JWT Laravel Package</t>
+  </si>
+  <si>
+    <t>117. Guard JWT</t>
+  </si>
+  <si>
+    <t>118. API Routes &amp; Middleware</t>
+  </si>
+  <si>
+    <t>119. API Login vía JWT</t>
+  </si>
+  <si>
+    <t>120. API Logout</t>
+  </si>
+  <si>
+    <t>https://github.com/JCarlosR/larajwt</t>
+  </si>
+  <si>
+    <t>Sección 15: Android: Consumir API</t>
+  </si>
+  <si>
+    <t>121. Especialidades, médicos por especialidad y horas</t>
+  </si>
+  <si>
+    <t>122. Introducción a Retrofit</t>
+  </si>
+  <si>
+    <t>123. Organización en Paquetes y ApiService</t>
+  </si>
+  <si>
+    <t>124. Primer llamado a la API</t>
+  </si>
+  <si>
+    <t>125. Spinner dependiente (médicos)</t>
+  </si>
+  <si>
+    <t>126. Horas según médico y fecha</t>
+  </si>
+  <si>
+    <t>127. Formato de fecha (mes que inicia en 0 o 1)</t>
+  </si>
+  <si>
+    <t>128. Mostrar horas y mensajes asociados</t>
+  </si>
+  <si>
+    <t>129. Inicio de sesión vía API y JSON Web Token</t>
+  </si>
+  <si>
+    <t>130. Cierre de sesión y Authorization Header</t>
+  </si>
+  <si>
+    <t>131. Citas médicas: modelo y formato JSON</t>
+  </si>
+  <si>
+    <t>132. Item appointment XML</t>
+  </si>
+  <si>
+    <t>133. AutoTransition para los CardView</t>
+  </si>
+  <si>
+    <t>134. Store Appointment (Refactorización)</t>
+  </si>
+  <si>
+    <t>135. Registro de cita médica (Android)</t>
+  </si>
+  <si>
+    <t>136. Refactorización: Registro Web y vía API</t>
+  </si>
+  <si>
+    <t>137. Registro desde Android</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="171" formatCode="[hh]:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,6 +548,14 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -415,10 +587,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -429,8 +602,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -451,16 +628,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Edenilson Ruiz" refreshedDate="43786.861996180553" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="93">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Edenilson Ruiz" refreshedDate="43793.740918171294" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="137">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabla1"/>
   </cacheSource>
-  <cacheFields count="5">
+  <cacheFields count="6">
     <cacheField name="SectionId" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="11"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="15"/>
     </cacheField>
     <cacheField name="SectionName" numFmtId="0">
-      <sharedItems count="17">
+      <sharedItems count="21">
         <s v="Sección 01: Introducción"/>
         <s v="Sección 02: Laravel: Configuración y Diseño Inicial"/>
         <s v="Sección 03: Laravel: Gestión de datos"/>
@@ -472,6 +649,10 @@
         <s v="Sección 09: Kotlin, como alternativa a Java"/>
         <s v="Sección 10: Android: DatePicker y otros detalles"/>
         <s v="Sección 11: Android: RecyclerView"/>
+        <s v="Sección 12: Android: Navegación entre pantallas"/>
+        <s v="Sección 13: Despliegue a producción"/>
+        <s v="Sección 14: Android y Laravel: Autenticación vía JWT"/>
+        <s v="Sección 15: Android: Consumir API"/>
         <s v="Sección 4: Laravel: Roles y seguridad" u="1"/>
         <s v="Sección 2: Laravel: Configuración y Diseño Inicial" u="1"/>
         <s v="Sección 3: Laravel: Gestión de datos" u="1"/>
@@ -481,10 +662,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="ClassNumber" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="93"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="137"/>
     </cacheField>
     <cacheField name="ClassName" numFmtId="0">
-      <sharedItems count="146">
+      <sharedItems count="190">
         <s v="01. Bienvenida y recomendaciones"/>
         <s v="02. Mockups (planteamiento inicial)"/>
         <s v="03. Laravel: Configuración Inicial"/>
@@ -578,6 +759,50 @@
         <s v="91. Item View XML &amp; DataSet"/>
         <s v="92. ViewHolder (Create &amp; Bind)"/>
         <s v="93. With y otros detalles"/>
+        <s v="94. Back button"/>
+        <s v="95. Finalizar un Activity tras iniciar otro"/>
+        <s v="96 Cómo tener una única instancia (Activity)"/>
+        <s v="97. Persistencia de datos para el Login"/>
+        <s v="98. Shared Preferences, tal como son"/>
+        <s v="99. Shared Preferences, usando Kotlin"/>
+        <s v="100. Repositorio en Github (Proyecto Android)"/>
+        <s v="101. Snackbar by lazy"/>
+        <s v="102. Alert Dialog"/>
+        <s v="103. Paso previo, mensaje de error y checked"/>
+        <s v="104. Mostrar datos, para Confirmar cita"/>
+        <s v="105. Validar selección de fecha y hora"/>
+        <s v="106. Off-topic: Cómo crear y compartir un Gif"/>
+        <s v="107. Registro en Digital Ocean"/>
+        <s v="108. Conexión vía SSH"/>
+        <s v="109. Instalación de paquetes y dependencias"/>
+        <s v="110. Corregir conexión MySQL"/>
+        <s v="111. Comandos Git: log, status, push, pull"/>
+        <s v="112. Laravel log"/>
+        <s v="113. Encoding, Encryption &amp; Hashing"/>
+        <s v="114. JWT: Flujo de autenticación"/>
+        <s v="115. Cómo se genera y valida un JWT (5 pasos)"/>
+        <s v="116. JWT Laravel Package"/>
+        <s v="117. Guard JWT"/>
+        <s v="118. API Routes &amp; Middleware"/>
+        <s v="119. API Login vía JWT"/>
+        <s v="120. API Logout"/>
+        <s v="121. Especialidades, médicos por especialidad y horas"/>
+        <s v="122. Introducción a Retrofit"/>
+        <s v="123. Organización en Paquetes y ApiService"/>
+        <s v="124. Primer llamado a la API"/>
+        <s v="125. Spinner dependiente (médicos)"/>
+        <s v="126. Horas según médico y fecha"/>
+        <s v="127. Formato de fecha (mes que inicia en 0 o 1)"/>
+        <s v="128. Mostrar horas y mensajes asociados"/>
+        <s v="129. Inicio de sesión vía API y JSON Web Token"/>
+        <s v="130. Cierre de sesión y Authorization Header"/>
+        <s v="131. Citas médicas: modelo y formato JSON"/>
+        <s v="132. Item appointment XML"/>
+        <s v="133. AutoTransition para los CardView"/>
+        <s v="134. Store Appointment (Refactorización)"/>
+        <s v="135. Registro de cita médica (Android)"/>
+        <s v="136. Refactorización: Registro Web y vía API"/>
+        <s v="137. Registro desde Android"/>
         <s v="Cancelación de citas médicas" u="1"/>
         <s v="Métodos update y destroy" u="1"/>
         <s v="Directiva include y menú lateral" u="1"/>
@@ -636,6 +861,9 @@
     <cacheField name="Time" numFmtId="21">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:02:00" maxDate="1899-12-30T01:05:00"/>
     </cacheField>
+    <cacheField name="Link" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -646,13 +874,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="93">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="137">
   <r>
     <n v="1"/>
     <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <d v="1899-12-30T00:03:00"/>
+    <m/>
   </r>
   <r>
     <n v="1"/>
@@ -660,6 +889,7 @@
     <n v="2"/>
     <x v="1"/>
     <d v="1899-12-30T00:11:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -667,6 +897,7 @@
     <n v="3"/>
     <x v="2"/>
     <d v="1899-12-30T00:11:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -674,6 +905,7 @@
     <n v="4"/>
     <x v="3"/>
     <d v="1899-12-30T00:06:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -681,6 +913,7 @@
     <n v="5"/>
     <x v="4"/>
     <d v="1899-12-30T00:02:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -688,6 +921,7 @@
     <n v="6"/>
     <x v="5"/>
     <d v="1899-12-30T00:07:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -695,6 +929,7 @@
     <n v="7"/>
     <x v="6"/>
     <d v="1899-12-30T00:31:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -702,6 +937,7 @@
     <n v="8"/>
     <x v="7"/>
     <d v="1899-12-30T00:09:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -709,6 +945,7 @@
     <n v="9"/>
     <x v="8"/>
     <d v="1899-12-30T00:11:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -716,6 +953,7 @@
     <n v="10"/>
     <x v="9"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -723,6 +961,7 @@
     <n v="11"/>
     <x v="10"/>
     <d v="1899-12-30T00:15:00"/>
+    <m/>
   </r>
   <r>
     <n v="2"/>
@@ -730,6 +969,7 @@
     <n v="12"/>
     <x v="11"/>
     <d v="1899-12-30T00:21:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -737,6 +977,7 @@
     <n v="13"/>
     <x v="12"/>
     <d v="1899-12-30T00:29:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -744,6 +985,7 @@
     <n v="14"/>
     <x v="13"/>
     <d v="1899-12-30T00:09:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -751,6 +993,7 @@
     <n v="15"/>
     <x v="14"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -758,6 +1001,7 @@
     <n v="16"/>
     <x v="15"/>
     <d v="1899-12-30T00:07:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -765,6 +1009,7 @@
     <n v="17"/>
     <x v="16"/>
     <d v="1899-12-30T00:10:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -772,6 +1017,7 @@
     <n v="18"/>
     <x v="17"/>
     <d v="1899-12-30T00:18:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -779,6 +1025,7 @@
     <n v="19"/>
     <x v="18"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -786,6 +1033,7 @@
     <n v="20"/>
     <x v="19"/>
     <d v="1899-12-30T00:11:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -793,6 +1041,7 @@
     <n v="21"/>
     <x v="20"/>
     <d v="1899-12-30T00:23:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -800,6 +1049,7 @@
     <n v="22"/>
     <x v="21"/>
     <d v="1899-12-30T00:09:00"/>
+    <m/>
   </r>
   <r>
     <n v="3"/>
@@ -807,6 +1057,7 @@
     <n v="23"/>
     <x v="22"/>
     <d v="1899-12-30T00:10:00"/>
+    <m/>
   </r>
   <r>
     <n v="4"/>
@@ -814,6 +1065,7 @@
     <n v="24"/>
     <x v="23"/>
     <d v="1899-12-30T00:11:00"/>
+    <m/>
   </r>
   <r>
     <n v="4"/>
@@ -821,6 +1073,7 @@
     <n v="25"/>
     <x v="24"/>
     <d v="1899-12-30T00:08:00"/>
+    <m/>
   </r>
   <r>
     <n v="4"/>
@@ -828,6 +1081,7 @@
     <n v="26"/>
     <x v="25"/>
     <d v="1899-12-30T00:04:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -835,6 +1089,7 @@
     <n v="27"/>
     <x v="26"/>
     <d v="1899-12-30T00:16:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -842,6 +1097,7 @@
     <n v="28"/>
     <x v="27"/>
     <d v="1899-12-30T00:25:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -849,6 +1105,7 @@
     <n v="29"/>
     <x v="28"/>
     <d v="1899-12-30T00:06:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -856,6 +1113,7 @@
     <n v="30"/>
     <x v="29"/>
     <d v="1899-12-30T00:16:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -863,6 +1121,7 @@
     <n v="31"/>
     <x v="30"/>
     <d v="1899-12-30T00:15:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -870,6 +1129,7 @@
     <n v="32"/>
     <x v="31"/>
     <d v="1899-12-30T00:12:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -877,6 +1137,7 @@
     <n v="33"/>
     <x v="32"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -884,6 +1145,7 @@
     <n v="34"/>
     <x v="33"/>
     <d v="1899-12-30T00:12:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -891,6 +1153,7 @@
     <n v="35"/>
     <x v="34"/>
     <d v="1899-12-30T00:16:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -898,6 +1161,7 @@
     <n v="36"/>
     <x v="35"/>
     <d v="1899-12-30T00:15:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -905,6 +1169,7 @@
     <n v="37"/>
     <x v="36"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -912,6 +1177,7 @@
     <n v="38"/>
     <x v="37"/>
     <d v="1899-12-30T00:31:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -919,6 +1185,7 @@
     <n v="39"/>
     <x v="38"/>
     <d v="1899-12-30T00:23:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -926,6 +1193,7 @@
     <n v="40"/>
     <x v="39"/>
     <d v="1899-12-30T01:05:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -933,6 +1201,7 @@
     <n v="41"/>
     <x v="40"/>
     <d v="1899-12-30T00:41:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -940,6 +1209,7 @@
     <n v="42"/>
     <x v="41"/>
     <d v="1899-12-30T00:08:00"/>
+    <m/>
   </r>
   <r>
     <n v="5"/>
@@ -947,6 +1217,7 @@
     <n v="43"/>
     <x v="42"/>
     <d v="1899-12-30T00:16:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -954,6 +1225,7 @@
     <n v="44"/>
     <x v="43"/>
     <d v="1899-12-30T00:25:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -961,6 +1233,7 @@
     <n v="45"/>
     <x v="44"/>
     <d v="1899-12-30T00:17:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -968,6 +1241,7 @@
     <n v="46"/>
     <x v="45"/>
     <d v="1899-12-30T00:20:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -975,6 +1249,7 @@
     <n v="47"/>
     <x v="46"/>
     <d v="1899-12-30T00:34:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -982,6 +1257,7 @@
     <n v="48"/>
     <x v="47"/>
     <d v="1899-12-30T00:20:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -989,6 +1265,7 @@
     <n v="49"/>
     <x v="48"/>
     <d v="1899-12-30T00:04:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -996,6 +1273,7 @@
     <n v="50"/>
     <x v="49"/>
     <d v="1899-12-30T00:18:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -1003,6 +1281,7 @@
     <n v="51"/>
     <x v="50"/>
     <d v="1899-12-30T00:06:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -1010,6 +1289,7 @@
     <n v="52"/>
     <x v="51"/>
     <d v="1899-12-30T00:10:00"/>
+    <m/>
   </r>
   <r>
     <n v="6"/>
@@ -1017,6 +1297,7 @@
     <n v="53"/>
     <x v="52"/>
     <d v="1899-12-30T00:16:00"/>
+    <m/>
   </r>
   <r>
     <n v="7"/>
@@ -1024,6 +1305,7 @@
     <n v="54"/>
     <x v="53"/>
     <d v="1899-12-30T00:09:00"/>
+    <m/>
   </r>
   <r>
     <n v="7"/>
@@ -1031,6 +1313,7 @@
     <n v="55"/>
     <x v="54"/>
     <d v="1899-12-30T00:26:00"/>
+    <m/>
   </r>
   <r>
     <n v="7"/>
@@ -1038,6 +1321,7 @@
     <n v="56"/>
     <x v="55"/>
     <d v="1899-12-30T00:41:00"/>
+    <m/>
   </r>
   <r>
     <n v="7"/>
@@ -1045,6 +1329,7 @@
     <n v="57"/>
     <x v="56"/>
     <d v="1899-12-30T00:19:00"/>
+    <m/>
   </r>
   <r>
     <n v="7"/>
@@ -1052,6 +1337,7 @@
     <n v="58"/>
     <x v="57"/>
     <d v="1899-12-30T00:12:00"/>
+    <m/>
   </r>
   <r>
     <n v="7"/>
@@ -1059,6 +1345,7 @@
     <n v="59"/>
     <x v="58"/>
     <d v="1899-12-30T00:28:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1066,6 +1353,7 @@
     <n v="60"/>
     <x v="59"/>
     <d v="1899-12-30T00:03:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1073,6 +1361,7 @@
     <n v="61"/>
     <x v="60"/>
     <d v="1899-12-30T00:10:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1080,6 +1369,7 @@
     <n v="62"/>
     <x v="61"/>
     <d v="1899-12-30T00:05:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1087,6 +1377,7 @@
     <n v="63"/>
     <x v="62"/>
     <d v="1899-12-30T00:06:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1094,6 +1385,7 @@
     <n v="64"/>
     <x v="63"/>
     <d v="1899-12-30T00:32:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1101,6 +1393,7 @@
     <n v="65"/>
     <x v="64"/>
     <d v="1899-12-30T00:21:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1108,6 +1401,7 @@
     <n v="66"/>
     <x v="65"/>
     <d v="1899-12-30T00:19:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1115,6 +1409,7 @@
     <n v="67"/>
     <x v="66"/>
     <d v="1899-12-30T00:16:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1122,6 +1417,7 @@
     <n v="68"/>
     <x v="67"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="8"/>
@@ -1129,6 +1425,7 @@
     <n v="69"/>
     <x v="68"/>
     <d v="1899-12-30T00:08:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1136,6 +1433,7 @@
     <n v="70"/>
     <x v="69"/>
     <d v="1899-12-30T00:10:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1143,6 +1441,7 @@
     <n v="71"/>
     <x v="70"/>
     <d v="1899-12-30T00:15:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1150,6 +1449,7 @@
     <n v="72"/>
     <x v="71"/>
     <d v="1899-12-30T00:27:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1157,6 +1457,7 @@
     <n v="73"/>
     <x v="72"/>
     <d v="1899-12-30T00:18:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1164,6 +1465,7 @@
     <n v="74"/>
     <x v="73"/>
     <d v="1899-12-30T00:12:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1171,6 +1473,7 @@
     <n v="75"/>
     <x v="74"/>
     <d v="1899-12-30T00:03:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1178,6 +1481,7 @@
     <n v="76"/>
     <x v="75"/>
     <d v="1899-12-30T00:12:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1185,6 +1489,7 @@
     <n v="77"/>
     <x v="76"/>
     <d v="1899-12-30T00:05:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1192,6 +1497,7 @@
     <n v="78"/>
     <x v="77"/>
     <d v="1899-12-30T00:11:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1199,6 +1505,7 @@
     <n v="79"/>
     <x v="78"/>
     <d v="1899-12-30T00:10:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1206,6 +1513,7 @@
     <n v="80"/>
     <x v="79"/>
     <d v="1899-12-30T00:15:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1213,6 +1521,7 @@
     <n v="81"/>
     <x v="80"/>
     <d v="1899-12-30T00:08:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1220,6 +1529,7 @@
     <n v="82"/>
     <x v="81"/>
     <d v="1899-12-30T00:13:00"/>
+    <m/>
   </r>
   <r>
     <n v="9"/>
@@ -1227,6 +1537,7 @@
     <n v="83"/>
     <x v="82"/>
     <d v="1899-12-30T00:25:00"/>
+    <m/>
   </r>
   <r>
     <n v="10"/>
@@ -1234,6 +1545,7 @@
     <n v="84"/>
     <x v="83"/>
     <d v="1899-12-30T00:15:00"/>
+    <m/>
   </r>
   <r>
     <n v="10"/>
@@ -1241,6 +1553,7 @@
     <n v="85"/>
     <x v="84"/>
     <d v="1899-12-30T00:02:00"/>
+    <m/>
   </r>
   <r>
     <n v="10"/>
@@ -1248,6 +1561,7 @@
     <n v="86"/>
     <x v="85"/>
     <d v="1899-12-30T00:05:00"/>
+    <m/>
   </r>
   <r>
     <n v="10"/>
@@ -1255,6 +1569,7 @@
     <n v="87"/>
     <x v="86"/>
     <d v="1899-12-30T00:03:00"/>
+    <m/>
   </r>
   <r>
     <n v="10"/>
@@ -1262,6 +1577,7 @@
     <n v="88"/>
     <x v="87"/>
     <d v="1899-12-30T00:18:00"/>
+    <m/>
   </r>
   <r>
     <n v="10"/>
@@ -1269,6 +1585,7 @@
     <n v="89"/>
     <x v="88"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="11"/>
@@ -1276,6 +1593,7 @@
     <n v="90"/>
     <x v="89"/>
     <d v="1899-12-30T00:14:00"/>
+    <m/>
   </r>
   <r>
     <n v="11"/>
@@ -1283,6 +1601,7 @@
     <n v="91"/>
     <x v="90"/>
     <d v="1899-12-30T00:22:00"/>
+    <m/>
   </r>
   <r>
     <n v="11"/>
@@ -1290,6 +1609,7 @@
     <n v="92"/>
     <x v="91"/>
     <d v="1899-12-30T00:10:00"/>
+    <m/>
   </r>
   <r>
     <n v="11"/>
@@ -1297,23 +1617,376 @@
     <n v="93"/>
     <x v="92"/>
     <d v="1899-12-30T00:12:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="94"/>
+    <x v="93"/>
+    <d v="1899-12-30T00:08:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="95"/>
+    <x v="94"/>
+    <d v="1899-12-30T00:02:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="96"/>
+    <x v="95"/>
+    <d v="1899-12-30T00:06:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="97"/>
+    <x v="96"/>
+    <d v="1899-12-30T00:07:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="98"/>
+    <x v="97"/>
+    <d v="1899-12-30T00:11:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="99"/>
+    <x v="98"/>
+    <d v="1899-12-30T00:24:00"/>
+    <s v="https://gist.github.com/JCarlosR/7f457aeebd9c3670933221e97116c4c6"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="100"/>
+    <x v="99"/>
+    <d v="1899-12-30T00:03:00"/>
+    <s v="https://github.com/JCarlosR/MyAppointments"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="101"/>
+    <x v="100"/>
+    <d v="1899-12-30T00:11:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="102"/>
+    <x v="101"/>
+    <d v="1899-12-30T00:09:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="103"/>
+    <x v="102"/>
+    <d v="1899-12-30T00:08:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="104"/>
+    <x v="103"/>
+    <d v="1899-12-30T00:36:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="105"/>
+    <x v="104"/>
+    <d v="1899-12-30T00:12:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="11"/>
+    <n v="106"/>
+    <x v="105"/>
+    <d v="1899-12-30T00:03:00"/>
+    <s v="Gifcam.zip"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="12"/>
+    <n v="107"/>
+    <x v="106"/>
+    <d v="1899-12-30T00:08:00"/>
+    <s v="https://programacionymas.com/blog/hacer-deploy-app-laravel-digital-ocean"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="12"/>
+    <n v="108"/>
+    <x v="107"/>
+    <d v="1899-12-30T00:02:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="12"/>
+    <n v="109"/>
+    <x v="108"/>
+    <d v="1899-12-30T00:18:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="12"/>
+    <n v="110"/>
+    <x v="109"/>
+    <d v="1899-12-30T00:03:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="12"/>
+    <n v="111"/>
+    <x v="110"/>
+    <d v="1899-12-30T00:06:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="12"/>
+    <n v="112"/>
+    <x v="111"/>
+    <d v="1899-12-30T00:07:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="113"/>
+    <x v="112"/>
+    <d v="1899-12-30T00:13:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="114"/>
+    <x v="113"/>
+    <d v="1899-12-30T00:08:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="115"/>
+    <x v="114"/>
+    <d v="1899-12-30T00:19:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="116"/>
+    <x v="115"/>
+    <d v="1899-12-30T00:07:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="117"/>
+    <x v="116"/>
+    <d v="1899-12-30T00:06:00"/>
+    <s v="https://github.com/JCarlosR/larajwt"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="118"/>
+    <x v="117"/>
+    <d v="1899-12-30T00:15:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="119"/>
+    <x v="118"/>
+    <d v="1899-12-30T00:12:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="13"/>
+    <n v="120"/>
+    <x v="119"/>
+    <d v="1899-12-30T00:06:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="121"/>
+    <x v="120"/>
+    <d v="1899-12-30T00:10:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="122"/>
+    <x v="121"/>
+    <d v="1899-12-30T00:05:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="123"/>
+    <x v="122"/>
+    <d v="1899-12-30T00:11:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="124"/>
+    <x v="123"/>
+    <d v="1899-12-30T00:19:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="125"/>
+    <x v="124"/>
+    <d v="1899-12-30T00:15:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="126"/>
+    <x v="125"/>
+    <d v="1899-12-30T00:22:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="127"/>
+    <x v="126"/>
+    <d v="1899-12-30T00:05:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="128"/>
+    <x v="127"/>
+    <d v="1899-12-30T00:17:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="129"/>
+    <x v="128"/>
+    <d v="1899-12-30T00:21:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="130"/>
+    <x v="129"/>
+    <d v="1899-12-30T00:17:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="131"/>
+    <x v="130"/>
+    <d v="1899-12-30T00:27:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="132"/>
+    <x v="131"/>
+    <d v="1899-12-30T00:16:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="133"/>
+    <x v="132"/>
+    <d v="1899-12-30T00:04:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="134"/>
+    <x v="133"/>
+    <d v="1899-12-30T00:27:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="135"/>
+    <x v="134"/>
+    <d v="1899-12-30T00:24:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="136"/>
+    <x v="135"/>
+    <d v="1899-12-30T00:25:00"/>
+    <m/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="14"/>
+    <n v="137"/>
+    <x v="136"/>
+    <d v="1899-12-30T00:17:00"/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Sección">
-  <location ref="B4:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
+  <location ref="B4:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="18">
+      <items count="22">
+        <item sd="0" m="1" x="19"/>
+        <item sd="0" m="1" x="16"/>
+        <item sd="0" m="1" x="17"/>
         <item sd="0" m="1" x="15"/>
-        <item sd="0" m="1" x="12"/>
-        <item sd="0" m="1" x="13"/>
-        <item sd="0" m="1" x="11"/>
-        <item sd="0" m="1" x="16"/>
-        <item sd="0" m="1" x="14"/>
+        <item sd="0" m="1" x="20"/>
+        <item sd="0" m="1" x="18"/>
         <item sd="0" x="0"/>
         <item sd="0" x="1"/>
         <item sd="0" x="2"/>
@@ -1325,65 +1998,69 @@
         <item sd="0" x="8"/>
         <item sd="0" x="9"/>
         <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
         <item t="default" sd="0"/>
       </items>
     </pivotField>
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="146">
+      <items count="190">
+        <item m="1" x="185"/>
+        <item m="1" x="187"/>
+        <item m="1" x="157"/>
+        <item m="1" x="137"/>
+        <item m="1" x="178"/>
+        <item m="1" x="151"/>
+        <item m="1" x="186"/>
+        <item m="1" x="140"/>
+        <item m="1" x="150"/>
+        <item m="1" x="188"/>
+        <item m="1" x="139"/>
+        <item m="1" x="162"/>
+        <item m="1" x="163"/>
+        <item m="1" x="184"/>
+        <item m="1" x="167"/>
+        <item m="1" x="174"/>
+        <item m="1" x="180"/>
+        <item m="1" x="149"/>
+        <item m="1" x="144"/>
+        <item m="1" x="158"/>
+        <item m="1" x="165"/>
+        <item m="1" x="172"/>
+        <item m="1" x="181"/>
+        <item m="1" x="170"/>
+        <item m="1" x="171"/>
+        <item m="1" x="168"/>
+        <item m="1" x="159"/>
+        <item m="1" x="146"/>
+        <item m="1" x="164"/>
+        <item m="1" x="138"/>
+        <item m="1" x="175"/>
+        <item m="1" x="182"/>
+        <item m="1" x="145"/>
+        <item m="1" x="169"/>
+        <item m="1" x="179"/>
+        <item m="1" x="155"/>
+        <item m="1" x="177"/>
+        <item m="1" x="156"/>
+        <item m="1" x="189"/>
+        <item m="1" x="153"/>
+        <item m="1" x="173"/>
         <item m="1" x="141"/>
+        <item m="1" x="160"/>
+        <item m="1" x="154"/>
+        <item m="1" x="183"/>
         <item m="1" x="143"/>
-        <item m="1" x="113"/>
-        <item m="1" x="93"/>
-        <item m="1" x="134"/>
-        <item m="1" x="107"/>
+        <item m="1" x="147"/>
+        <item m="1" x="148"/>
+        <item m="1" x="166"/>
+        <item m="1" x="176"/>
+        <item m="1" x="152"/>
         <item m="1" x="142"/>
-        <item m="1" x="96"/>
-        <item m="1" x="106"/>
-        <item m="1" x="144"/>
-        <item m="1" x="95"/>
-        <item m="1" x="118"/>
-        <item m="1" x="119"/>
-        <item m="1" x="140"/>
-        <item m="1" x="123"/>
-        <item m="1" x="130"/>
-        <item m="1" x="136"/>
-        <item m="1" x="105"/>
-        <item m="1" x="100"/>
-        <item m="1" x="114"/>
-        <item m="1" x="121"/>
-        <item m="1" x="128"/>
-        <item m="1" x="137"/>
-        <item m="1" x="126"/>
-        <item m="1" x="127"/>
-        <item m="1" x="124"/>
-        <item m="1" x="115"/>
-        <item m="1" x="102"/>
-        <item m="1" x="120"/>
-        <item m="1" x="94"/>
-        <item m="1" x="131"/>
-        <item m="1" x="138"/>
-        <item m="1" x="101"/>
-        <item m="1" x="125"/>
-        <item m="1" x="135"/>
-        <item m="1" x="111"/>
-        <item m="1" x="133"/>
-        <item m="1" x="112"/>
-        <item m="1" x="145"/>
-        <item m="1" x="109"/>
-        <item m="1" x="129"/>
-        <item m="1" x="97"/>
-        <item m="1" x="116"/>
-        <item m="1" x="110"/>
-        <item m="1" x="139"/>
-        <item m="1" x="99"/>
-        <item m="1" x="103"/>
-        <item m="1" x="104"/>
-        <item m="1" x="122"/>
-        <item m="1" x="132"/>
-        <item m="1" x="108"/>
-        <item m="1" x="98"/>
-        <item m="1" x="117"/>
+        <item m="1" x="161"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1477,15 +2154,60 @@
         <item x="90"/>
         <item x="91"/>
         <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
       </items>
     </pivotField>
     <pivotField dataField="1" numFmtId="21" showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="1"/>
     <field x="3"/>
   </rowFields>
-  <rowItems count="12">
+  <rowItems count="16">
     <i>
       <x v="6"/>
     </i>
@@ -1519,6 +2241,18 @@
     <i>
       <x v="16"/>
     </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -1527,7 +2261,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="TiempoInvertido" fld="4" baseField="1" baseItem="0" numFmtId="164"/>
+    <dataField name="TiempoInvertido" fld="4" baseField="1" baseItem="14" numFmtId="171"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight13" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1539,13 +2273,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E94" totalsRowShown="0">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F138" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="1" name="SectionId"/>
     <tableColumn id="5" name="SectionName"/>
     <tableColumn id="2" name="ClassNumber"/>
     <tableColumn id="4" name="ClassName"/>
     <tableColumn id="3" name="Time" dataDxfId="0"/>
+    <tableColumn id="6" name="Link"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1838,16 +2573,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C16"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="51" width="8.140625" customWidth="1"/>
     <col min="52" max="52" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -1871,7 +2604,7 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="8">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
@@ -1879,7 +2612,7 @@
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="8">
         <v>8.819444444444445E-2</v>
       </c>
     </row>
@@ -1887,7 +2620,7 @@
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="8">
         <v>0.10694444444444445</v>
       </c>
     </row>
@@ -1895,7 +2628,7 @@
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="8">
         <v>1.5972222222222221E-2</v>
       </c>
     </row>
@@ -1903,7 +2636,7 @@
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="8">
         <v>0.23958333333333334</v>
       </c>
     </row>
@@ -1911,7 +2644,7 @@
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="8">
         <v>0.11805555555555555</v>
       </c>
     </row>
@@ -1919,7 +2652,7 @@
       <c r="B11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="8">
         <v>9.375E-2</v>
       </c>
     </row>
@@ -1927,7 +2660,7 @@
       <c r="B12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="8">
         <v>9.3055555555555544E-2</v>
       </c>
     </row>
@@ -1935,7 +2668,7 @@
       <c r="B13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="8">
         <v>0.12777777777777777</v>
       </c>
     </row>
@@ -1943,7 +2676,7 @@
       <c r="B14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="8">
         <v>3.9583333333333331E-2</v>
       </c>
     </row>
@@ -1951,17 +2684,50 @@
       <c r="B15" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="8">
         <v>4.0277777777777773E-2</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="8">
+        <v>9.7222222222222224E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="8">
+        <v>3.0555555555555555E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5.9722222222222211E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.1958333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4">
-        <v>0.97291666666666665</v>
-      </c>
+      <c r="C20" s="8">
+        <v>1.35625</v>
+      </c>
+      <c r="E20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1974,22 +2740,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView showGridLines="0" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2005,8 +2772,11 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2023,7 +2793,7 @@
         <v>2.0833333333333333E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2040,7 +2810,7 @@
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2057,7 +2827,7 @@
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2074,7 +2844,7 @@
         <v>4.1666666666666666E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2091,7 +2861,7 @@
         <v>1.3888888888888889E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2108,7 +2878,7 @@
         <v>4.8611111111111112E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2125,7 +2895,7 @@
         <v>2.1527777777777781E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2142,7 +2912,7 @@
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2159,7 +2929,7 @@
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2176,7 +2946,7 @@
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2193,7 +2963,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2210,7 +2980,7 @@
         <v>1.4583333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2227,7 +2997,7 @@
         <v>2.013888888888889E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2244,7 +3014,7 @@
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3587,10 +4357,795 @@
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>12</v>
+      </c>
+      <c r="B95" t="s">
+        <v>113</v>
+      </c>
+      <c r="C95">
+        <v>94</v>
+      </c>
+      <c r="D95" t="s">
+        <v>114</v>
+      </c>
+      <c r="E95" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>12</v>
+      </c>
+      <c r="B96" t="s">
+        <v>113</v>
+      </c>
+      <c r="C96">
+        <v>95</v>
+      </c>
+      <c r="D96" t="s">
+        <v>115</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>12</v>
+      </c>
+      <c r="B97" t="s">
+        <v>113</v>
+      </c>
+      <c r="C97">
+        <v>96</v>
+      </c>
+      <c r="D97" t="s">
+        <v>116</v>
+      </c>
+      <c r="E97" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>12</v>
+      </c>
+      <c r="B98" t="s">
+        <v>113</v>
+      </c>
+      <c r="C98">
+        <v>97</v>
+      </c>
+      <c r="D98" t="s">
+        <v>117</v>
+      </c>
+      <c r="E98" s="1">
+        <v>4.8611111111111112E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>12</v>
+      </c>
+      <c r="B99" t="s">
+        <v>113</v>
+      </c>
+      <c r="C99">
+        <v>98</v>
+      </c>
+      <c r="D99" t="s">
+        <v>119</v>
+      </c>
+      <c r="E99" s="1">
+        <v>7.6388888888888886E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>12</v>
+      </c>
+      <c r="B100" t="s">
+        <v>113</v>
+      </c>
+      <c r="C100">
+        <v>99</v>
+      </c>
+      <c r="D100" t="s">
+        <v>118</v>
+      </c>
+      <c r="E100" s="1">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>12</v>
+      </c>
+      <c r="B101" t="s">
+        <v>113</v>
+      </c>
+      <c r="C101">
+        <v>100</v>
+      </c>
+      <c r="D101" t="s">
+        <v>120</v>
+      </c>
+      <c r="E101" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>12</v>
+      </c>
+      <c r="B102" t="s">
+        <v>113</v>
+      </c>
+      <c r="C102">
+        <v>101</v>
+      </c>
+      <c r="D102" t="s">
+        <v>124</v>
+      </c>
+      <c r="E102" s="1">
+        <v>7.6388888888888886E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>12</v>
+      </c>
+      <c r="B103" t="s">
+        <v>113</v>
+      </c>
+      <c r="C103">
+        <v>102</v>
+      </c>
+      <c r="D103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E103" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>12</v>
+      </c>
+      <c r="B104" t="s">
+        <v>113</v>
+      </c>
+      <c r="C104">
+        <v>103</v>
+      </c>
+      <c r="D104" t="s">
+        <v>126</v>
+      </c>
+      <c r="E104" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>12</v>
+      </c>
+      <c r="B105" t="s">
+        <v>113</v>
+      </c>
+      <c r="C105">
+        <v>104</v>
+      </c>
+      <c r="D105" t="s">
+        <v>127</v>
+      </c>
+      <c r="E105" s="1">
+        <v>2.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>12</v>
+      </c>
+      <c r="B106" t="s">
+        <v>113</v>
+      </c>
+      <c r="C106">
+        <v>105</v>
+      </c>
+      <c r="D106" t="s">
+        <v>128</v>
+      </c>
+      <c r="E106" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>12</v>
+      </c>
+      <c r="B107" t="s">
+        <v>113</v>
+      </c>
+      <c r="C107">
+        <v>106</v>
+      </c>
+      <c r="D107" t="s">
+        <v>129</v>
+      </c>
+      <c r="E107" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="F107" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>13</v>
+      </c>
+      <c r="B108" t="s">
+        <v>131</v>
+      </c>
+      <c r="C108">
+        <v>107</v>
+      </c>
+      <c r="D108" t="s">
+        <v>132</v>
+      </c>
+      <c r="E108" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>13</v>
+      </c>
+      <c r="B109" t="s">
+        <v>131</v>
+      </c>
+      <c r="C109">
+        <v>108</v>
+      </c>
+      <c r="D109" t="s">
+        <v>134</v>
+      </c>
+      <c r="E109" s="1">
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>13</v>
+      </c>
+      <c r="B110" t="s">
+        <v>131</v>
+      </c>
+      <c r="C110">
+        <v>109</v>
+      </c>
+      <c r="D110" t="s">
+        <v>135</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>13</v>
+      </c>
+      <c r="B111" t="s">
+        <v>131</v>
+      </c>
+      <c r="C111">
+        <v>110</v>
+      </c>
+      <c r="D111" t="s">
+        <v>136</v>
+      </c>
+      <c r="E111" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>13</v>
+      </c>
+      <c r="B112" t="s">
+        <v>131</v>
+      </c>
+      <c r="C112">
+        <v>111</v>
+      </c>
+      <c r="D112" t="s">
+        <v>137</v>
+      </c>
+      <c r="E112" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>13</v>
+      </c>
+      <c r="B113" t="s">
+        <v>131</v>
+      </c>
+      <c r="C113">
+        <v>112</v>
+      </c>
+      <c r="D113" t="s">
+        <v>138</v>
+      </c>
+      <c r="E113" s="1">
+        <v>4.8611111111111112E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>14</v>
+      </c>
+      <c r="B114" t="s">
+        <v>139</v>
+      </c>
+      <c r="C114">
+        <v>113</v>
+      </c>
+      <c r="D114" t="s">
+        <v>140</v>
+      </c>
+      <c r="E114" s="1">
+        <v>9.0277777777777787E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>14</v>
+      </c>
+      <c r="B115" t="s">
+        <v>139</v>
+      </c>
+      <c r="C115">
+        <v>114</v>
+      </c>
+      <c r="D115" t="s">
+        <v>141</v>
+      </c>
+      <c r="E115" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>14</v>
+      </c>
+      <c r="B116" t="s">
+        <v>139</v>
+      </c>
+      <c r="C116">
+        <v>115</v>
+      </c>
+      <c r="D116" t="s">
+        <v>142</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1.3194444444444444E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>14</v>
+      </c>
+      <c r="B117" t="s">
+        <v>139</v>
+      </c>
+      <c r="C117">
+        <v>116</v>
+      </c>
+      <c r="D117" t="s">
+        <v>143</v>
+      </c>
+      <c r="E117" s="1">
+        <v>4.8611111111111112E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>14</v>
+      </c>
+      <c r="B118" t="s">
+        <v>139</v>
+      </c>
+      <c r="C118">
+        <v>117</v>
+      </c>
+      <c r="D118" t="s">
+        <v>144</v>
+      </c>
+      <c r="E118" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="F118" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>14</v>
+      </c>
+      <c r="B119" t="s">
+        <v>139</v>
+      </c>
+      <c r="C119">
+        <v>118</v>
+      </c>
+      <c r="D119" t="s">
+        <v>145</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>14</v>
+      </c>
+      <c r="B120" t="s">
+        <v>139</v>
+      </c>
+      <c r="C120">
+        <v>119</v>
+      </c>
+      <c r="D120" t="s">
+        <v>146</v>
+      </c>
+      <c r="E120" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>14</v>
+      </c>
+      <c r="B121" t="s">
+        <v>139</v>
+      </c>
+      <c r="C121">
+        <v>120</v>
+      </c>
+      <c r="D121" t="s">
+        <v>147</v>
+      </c>
+      <c r="E121" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>15</v>
+      </c>
+      <c r="B122" t="s">
+        <v>149</v>
+      </c>
+      <c r="C122">
+        <v>121</v>
+      </c>
+      <c r="D122" t="s">
+        <v>150</v>
+      </c>
+      <c r="E122" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="I122" s="7"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>15</v>
+      </c>
+      <c r="B123" t="s">
+        <v>149</v>
+      </c>
+      <c r="C123">
+        <v>122</v>
+      </c>
+      <c r="D123" t="s">
+        <v>151</v>
+      </c>
+      <c r="E123" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I123" s="7"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>15</v>
+      </c>
+      <c r="B124" t="s">
+        <v>149</v>
+      </c>
+      <c r="C124">
+        <v>123</v>
+      </c>
+      <c r="D124" t="s">
+        <v>152</v>
+      </c>
+      <c r="E124" s="1">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="I124" s="7"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>15</v>
+      </c>
+      <c r="B125" t="s">
+        <v>149</v>
+      </c>
+      <c r="C125">
+        <v>124</v>
+      </c>
+      <c r="D125" t="s">
+        <v>153</v>
+      </c>
+      <c r="E125" s="1">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="I125" s="7"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>15</v>
+      </c>
+      <c r="B126" t="s">
+        <v>149</v>
+      </c>
+      <c r="C126">
+        <v>125</v>
+      </c>
+      <c r="D126" t="s">
+        <v>154</v>
+      </c>
+      <c r="E126" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="I126" s="7"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>15</v>
+      </c>
+      <c r="B127" t="s">
+        <v>149</v>
+      </c>
+      <c r="C127">
+        <v>126</v>
+      </c>
+      <c r="D127" t="s">
+        <v>155</v>
+      </c>
+      <c r="E127" s="1">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="I127" s="7"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>15</v>
+      </c>
+      <c r="B128" t="s">
+        <v>149</v>
+      </c>
+      <c r="C128">
+        <v>127</v>
+      </c>
+      <c r="D128" t="s">
+        <v>156</v>
+      </c>
+      <c r="E128" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I128" s="7"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>15</v>
+      </c>
+      <c r="B129" t="s">
+        <v>149</v>
+      </c>
+      <c r="C129">
+        <v>128</v>
+      </c>
+      <c r="D129" t="s">
+        <v>157</v>
+      </c>
+      <c r="E129" s="1">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="I129" s="7"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>15</v>
+      </c>
+      <c r="B130" t="s">
+        <v>149</v>
+      </c>
+      <c r="C130">
+        <v>129</v>
+      </c>
+      <c r="D130" t="s">
+        <v>158</v>
+      </c>
+      <c r="E130" s="1">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="I130" s="7"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>15</v>
+      </c>
+      <c r="B131" t="s">
+        <v>149</v>
+      </c>
+      <c r="C131">
+        <v>130</v>
+      </c>
+      <c r="D131" t="s">
+        <v>159</v>
+      </c>
+      <c r="E131" s="1">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="I131" s="7"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>15</v>
+      </c>
+      <c r="B132" t="s">
+        <v>149</v>
+      </c>
+      <c r="C132">
+        <v>131</v>
+      </c>
+      <c r="D132" t="s">
+        <v>160</v>
+      </c>
+      <c r="E132" s="1">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="I132" s="7"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>15</v>
+      </c>
+      <c r="B133" t="s">
+        <v>149</v>
+      </c>
+      <c r="C133">
+        <v>132</v>
+      </c>
+      <c r="D133" t="s">
+        <v>161</v>
+      </c>
+      <c r="E133" s="1">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="I133" s="7"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>15</v>
+      </c>
+      <c r="B134" t="s">
+        <v>149</v>
+      </c>
+      <c r="C134">
+        <v>133</v>
+      </c>
+      <c r="D134" t="s">
+        <v>162</v>
+      </c>
+      <c r="E134" s="1">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I134" s="7"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>15</v>
+      </c>
+      <c r="B135" t="s">
+        <v>149</v>
+      </c>
+      <c r="C135">
+        <v>134</v>
+      </c>
+      <c r="D135" t="s">
+        <v>163</v>
+      </c>
+      <c r="E135" s="1">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="I135" s="7"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>15</v>
+      </c>
+      <c r="B136" t="s">
+        <v>149</v>
+      </c>
+      <c r="C136">
+        <v>135</v>
+      </c>
+      <c r="D136" t="s">
+        <v>164</v>
+      </c>
+      <c r="E136" s="1">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I136" s="7"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>15</v>
+      </c>
+      <c r="B137" t="s">
+        <v>149</v>
+      </c>
+      <c r="C137">
+        <v>136</v>
+      </c>
+      <c r="D137" t="s">
+        <v>165</v>
+      </c>
+      <c r="E137" s="1">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="I137" s="7"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>15</v>
+      </c>
+      <c r="B138" t="s">
+        <v>149</v>
+      </c>
+      <c r="C138">
+        <v>137</v>
+      </c>
+      <c r="D138" t="s">
+        <v>166</v>
+      </c>
+      <c r="E138" s="1">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="I138" s="7"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F101" r:id="rId1"/>
+    <hyperlink ref="F100" r:id="rId2"/>
+    <hyperlink ref="F108" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>